<commit_message>
refactor get_profile_all() in CostMaster to remove handling of no baselines. minor refactor of group_cost_profile_graph()
</commit_message>
<xml_diff>
--- a/tests/resources/cost_test_master_4_2019.xlsx
+++ b/tests/resources/cost_test_master_4_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="425">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -1503,7 +1503,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1602,7 +1602,9 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">

</xml_diff>